<commit_message>
mise à jour des taches
</commit_message>
<xml_diff>
--- a/Matlab_Contenu_Detaille.xlsx
+++ b/Matlab_Contenu_Detaille.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\Github\MATLAB_projet_echantillonage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marion\Desktop\Github\MATLAB_projet_echantillonage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A8C1B3-36A0-400E-A17F-EC90EC033DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27A079A-1EAB-4E38-B64F-6FEF1A20D964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planning" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="105">
   <si>
     <t>Environnement Matlab et types de fenêtres (Workspace, fenêtre de commande, …)</t>
   </si>
@@ -282,9 +282,6 @@
     <t>création du menu de lancement et des interface</t>
   </si>
   <si>
-    <t>Manipulation du bitshift</t>
-  </si>
-  <si>
     <t>fonction : moyenne entre Deux echantillons</t>
   </si>
   <si>
@@ -310,6 +307,57 @@
   </si>
   <si>
     <t>interp.m</t>
+  </si>
+  <si>
+    <t>Manipulation du bitshift Zero-padding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personne 1 </t>
+  </si>
+  <si>
+    <t>Personne 2</t>
+  </si>
+  <si>
+    <t>NON</t>
+  </si>
+  <si>
+    <t>aucun interet pour le projet finalement</t>
+  </si>
+  <si>
+    <t>Manipulation du bitshift lineaire</t>
+  </si>
+  <si>
+    <t>bit_delete.m</t>
+  </si>
+  <si>
+    <t>Manipulation du bitshift interpolation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation de la fonction zero-padding </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation de la fonction linaire </t>
+  </si>
+  <si>
+    <t xml:space="preserve">developpement partiellle sur la branche marion </t>
+  </si>
+  <si>
+    <t>developpement partiel sur la branche marion</t>
+  </si>
+  <si>
+    <t>OUI (branche marion)</t>
+  </si>
+  <si>
+    <t>Netoyage du code</t>
+  </si>
+  <si>
+    <t>Validation des fonctionnalités globales</t>
+  </si>
+  <si>
+    <t>developpement complet sur branche marion</t>
+  </si>
+  <si>
+    <t>developpement complet sur la branche marion</t>
   </si>
 </sst>
 </file>
@@ -417,7 +465,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -772,11 +820,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -823,6 +939,54 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -841,6 +1005,40 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -849,138 +1047,68 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color theme="9" tint="-0.499984740745262"/>
@@ -1013,11 +1141,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color theme="5" tint="-0.499984740745262"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1319,18 +1447,18 @@
       <c r="B4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="16" t="s">
+      <c r="D4" s="33"/>
+      <c r="E4" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="16" t="s">
+      <c r="F4" s="33"/>
+      <c r="G4" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="17"/>
+      <c r="H4" s="33"/>
       <c r="I4" s="13" t="s">
         <v>20</v>
       </c>
@@ -1342,19 +1470,19 @@
       <c r="B5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="20" t="s">
+      <c r="D5" s="37"/>
+      <c r="E5" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="20" t="s">
+      <c r="F5" s="37"/>
+      <c r="G5" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="26" t="s">
+      <c r="H5" s="37"/>
+      <c r="I5" s="45" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="14" t="s">
@@ -1365,19 +1493,19 @@
       <c r="B6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="29" t="s">
+      <c r="D6" s="37"/>
+      <c r="E6" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="37"/>
-      <c r="G6" s="22" t="s">
+      <c r="F6" s="39"/>
+      <c r="G6" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="27"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="46"/>
       <c r="J6" s="15" t="s">
         <v>24</v>
       </c>
@@ -1386,18 +1514,18 @@
       <c r="B7" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="37"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="22" t="s">
+      <c r="D7" s="39"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="23"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="29" t="s">
+      <c r="H7" s="55"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="42" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1405,37 +1533,37 @@
       <c r="B8" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="30"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="48"/>
     </row>
     <row r="9" spans="2:10" ht="18" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="18" t="s">
+      <c r="D9" s="35"/>
+      <c r="E9" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="18" t="s">
+      <c r="F9" s="35"/>
+      <c r="G9" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="31" t="s">
+      <c r="H9" s="35"/>
+      <c r="I9" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="34" t="s">
+      <c r="J9" s="52" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1461,8 +1589,8 @@
       <c r="H10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="32"/>
-      <c r="J10" s="35"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="53"/>
     </row>
     <row r="11" spans="2:10" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="12" t="s">
@@ -1486,7 +1614,7 @@
       <c r="H11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="33"/>
+      <c r="I11" s="51"/>
       <c r="J11" s="8" t="s">
         <v>40</v>
       </c>
@@ -1529,6 +1657,16 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H8"/>
+    <mergeCell ref="I5:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="E9:F9"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E4:F4"/>
@@ -1538,16 +1676,6 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F8"/>
-    <mergeCell ref="I5:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1556,301 +1684,515 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{883C19B0-CCFC-48B4-9B7E-E834A0101326}">
-  <dimension ref="B1:K13"/>
+  <dimension ref="B1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" customWidth="1"/>
-    <col min="4" max="6" width="25.7109375" customWidth="1"/>
-    <col min="7" max="10" width="15.7109375" customWidth="1"/>
-    <col min="11" max="11" width="50.7109375" customWidth="1"/>
+    <col min="2" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="50.7109375" customWidth="1"/>
+    <col min="5" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="42" t="s">
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="44"/>
-    </row>
-    <row r="3" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="46" t="s">
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="60"/>
+    </row>
+    <row r="3" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="E3" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="F3" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="G3" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="H3" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="I3" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="J3" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="46" t="s">
+      <c r="K3" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="K3" s="47" t="s">
+      <c r="L3" s="18" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="60" t="s">
+    <row r="4" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="31"/>
+      <c r="D4" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="53" t="s">
+      <c r="E4" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="F4" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="G4" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="53" t="s">
+      <c r="H4" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="H4" s="57">
+      <c r="I4" s="26">
         <v>44643</v>
       </c>
-      <c r="I4" s="57">
+      <c r="J4" s="26">
         <v>44655</v>
       </c>
-      <c r="J4" s="53" t="s">
+      <c r="K4" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="K4" s="54" t="s">
+      <c r="L4" s="62" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="60" t="s">
+    <row r="5" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="68"/>
+      <c r="D5" s="69" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="53" t="s">
+      <c r="E5" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="F5" s="70" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="53" t="s">
+      <c r="G5" s="70" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="53" t="s">
+      <c r="H5" s="70" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="57">
+      <c r="I5" s="71">
         <v>44615</v>
       </c>
-      <c r="I5" s="57">
+      <c r="J5" s="71">
         <v>44655</v>
       </c>
-      <c r="J5" s="53" t="s">
+      <c r="K5" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="K5" s="54" t="s">
+      <c r="L5" s="72" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="60"/>
-      <c r="C6" s="58" t="s">
+    <row r="6" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" s="26">
+        <v>44615</v>
+      </c>
+      <c r="J6" s="26">
+        <v>44703</v>
+      </c>
+      <c r="K6" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="L6" s="62"/>
+    </row>
+    <row r="7" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="26">
+        <v>44615</v>
+      </c>
+      <c r="J7" s="26">
+        <v>44703</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="L7" s="62"/>
+    </row>
+    <row r="8" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="69" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="70" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="70" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="70"/>
+      <c r="H8" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="71">
+        <v>44703</v>
+      </c>
+      <c r="J8" s="71"/>
+      <c r="K8" s="68"/>
+      <c r="L8" s="72"/>
+    </row>
+    <row r="9" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="73"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="65" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53" t="s">
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="74">
+        <v>44615</v>
+      </c>
+      <c r="J9" s="66"/>
+      <c r="K9" s="64" t="s">
+        <v>91</v>
+      </c>
+      <c r="L9" s="75" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="31"/>
+      <c r="D10" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="26">
+        <v>44615</v>
+      </c>
+      <c r="J10" s="26">
+        <v>44691</v>
+      </c>
+      <c r="K10" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="L10" s="62" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="31"/>
+      <c r="D11" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="26">
+        <v>44615</v>
+      </c>
+      <c r="J11" s="26">
+        <v>44662</v>
+      </c>
+      <c r="K11" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="L11" s="62" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="69" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="70" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="70"/>
+      <c r="H12" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="I12" s="71">
+        <v>44703</v>
+      </c>
+      <c r="J12" s="71"/>
+      <c r="K12" s="68"/>
+      <c r="L12" s="72"/>
+    </row>
+    <row r="13" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" s="26">
+        <v>44691</v>
+      </c>
+      <c r="J13" s="24"/>
+      <c r="K13" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="L13" s="62" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="26">
+        <v>44691</v>
+      </c>
+      <c r="J14" s="24"/>
+      <c r="K14" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="L14" s="62" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="67" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="69"/>
+      <c r="E15" s="70" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="70"/>
+      <c r="H15" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="54"/>
-    </row>
-    <row r="7" spans="2:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="60"/>
-      <c r="C7" s="58" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53" t="s">
+      <c r="I15" s="71">
+        <v>44703</v>
+      </c>
+      <c r="J15" s="70"/>
+      <c r="K15" s="68"/>
+      <c r="L15" s="72"/>
+    </row>
+    <row r="16" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="H7" s="57">
-        <v>44615</v>
-      </c>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="54"/>
-    </row>
-    <row r="8" spans="2:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="60"/>
-      <c r="C8" s="58" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="53" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="53" t="s">
-        <v>82</v>
-      </c>
-      <c r="G8" s="53" t="s">
+      <c r="I16" s="26">
+        <v>44703</v>
+      </c>
+      <c r="J16" s="24"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="62"/>
+    </row>
+    <row r="17" spans="2:12" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="H17" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="H8" s="57">
-        <v>44615</v>
-      </c>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="54"/>
-    </row>
-    <row r="9" spans="2:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="53" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="53" t="s">
-        <v>84</v>
-      </c>
-      <c r="G9" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="H9" s="57">
-        <v>44615</v>
-      </c>
-      <c r="I9" s="57">
-        <v>44662</v>
-      </c>
-      <c r="J9" s="62" t="s">
-        <v>85</v>
-      </c>
-      <c r="K9" s="54"/>
-    </row>
-    <row r="10" spans="2:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="60"/>
-      <c r="C10" s="58" t="s">
-        <v>86</v>
-      </c>
-      <c r="D10" s="53" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" s="53" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10" s="53" t="s">
-        <v>88</v>
-      </c>
-      <c r="G10" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="54"/>
-    </row>
-    <row r="11" spans="2:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="60"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="54"/>
-    </row>
-    <row r="12" spans="2:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="60"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="54"/>
-    </row>
-    <row r="13" spans="2:11" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="61"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="56"/>
+      <c r="I17" s="76">
+        <v>44703</v>
+      </c>
+      <c r="J17" s="25"/>
+      <c r="K17" s="61"/>
+      <c r="L17" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B2:L2"/>
   </mergeCells>
-  <conditionalFormatting sqref="G4:G13">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+  <conditionalFormatting sqref="H4:H17">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"en cours"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"bloque"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>"en cours"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B13" xr:uid="{D9C5B7B4-9BEC-465F-A75F-1BB3600E899E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C17" xr:uid="{D9C5B7B4-9BEC-465F-A75F-1BB3600E899E}">
       <formula1>personne</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D13" xr:uid="{5090458F-F807-4B1B-AB19-836F48BBE046}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E17" xr:uid="{5090458F-F807-4B1B-AB19-836F48BBE046}">
       <formula1>mode</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E13" xr:uid="{7DC4FA1D-567B-4F7F-AE97-F37D1D4DF8FB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F17" xr:uid="{7DC4FA1D-567B-4F7F-AE97-F37D1D4DF8FB}">
       <formula1>fonction</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G13" xr:uid="{74230D5F-4C46-4F6D-91AB-1AF8903CC68C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H17" xr:uid="{74230D5F-4C46-4F6D-91AB-1AF8903CC68C}">
       <formula1>etat</formula1>
     </dataValidation>
   </dataValidations>
@@ -1860,8 +2202,22 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{97A9259C-7E98-4C75-803D-D21BE7256BA9}">
+            <xm:f>NOT(ISERROR(SEARCH(Setting!$F$3,H4)))</xm:f>
+            <xm:f>Setting!$F$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
           <x14:cfRule type="containsText" priority="4" operator="containsText" id="{E59222D6-6A95-41C5-9D5F-A0D87D70219E}">
-            <xm:f>NOT(ISERROR(SEARCH("finis",G4)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH("finis",H4)))</xm:f>
             <xm:f>"finis"</xm:f>
             <x14:dxf>
               <font>
@@ -1874,21 +2230,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{97A9259C-7E98-4C75-803D-D21BE7256BA9}">
-            <xm:f>NOT(ISERROR(SEARCH(Setting!$F$3,G4)))</xm:f>
-            <xm:f>Setting!$F$3</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>G4:G13</xm:sqref>
+          <xm:sqref>H4:H17</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1911,80 +2253,80 @@
   <sheetData>
     <row r="1" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="3:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="22" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="52" t="s">
+      <c r="F3" s="23" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="23" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="49" t="s">
+      <c r="E5" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="49" t="s">
+      <c r="F5" s="20" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49" t="s">
+      <c r="D6" s="20"/>
+      <c r="E6" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="49" t="s">
+      <c r="F6" s="20" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
leger modif pour yohann
</commit_message>
<xml_diff>
--- a/Matlab_Contenu_Detaille.xlsx
+++ b/Matlab_Contenu_Detaille.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marion\Desktop\Github\MATLAB_projet_echantillonage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27A079A-1EAB-4E38-B64F-6FEF1A20D964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1B571B-22B2-4552-8909-3193BE3C3692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="106">
   <si>
     <t>Environnement Matlab et types de fenêtres (Workspace, fenêtre de commande, …)</t>
   </si>
@@ -358,6 +358,9 @@
   </si>
   <si>
     <t>developpement complet sur la branche marion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation de la fonction interpolation </t>
   </si>
 </sst>
 </file>
@@ -987,6 +990,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1005,6 +1056,34 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1017,36 +1096,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1054,54 +1105,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1447,18 +1450,18 @@
       <c r="B4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="32" t="s">
+      <c r="D4" s="49"/>
+      <c r="E4" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="33"/>
-      <c r="G4" s="32" t="s">
+      <c r="F4" s="49"/>
+      <c r="G4" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="33"/>
+      <c r="H4" s="49"/>
       <c r="I4" s="13" t="s">
         <v>20</v>
       </c>
@@ -1470,19 +1473,19 @@
       <c r="B5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="36" t="s">
+      <c r="D5" s="53"/>
+      <c r="E5" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="37"/>
-      <c r="G5" s="36" t="s">
+      <c r="F5" s="53"/>
+      <c r="G5" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="37"/>
-      <c r="I5" s="45" t="s">
+      <c r="H5" s="53"/>
+      <c r="I5" s="58" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="14" t="s">
@@ -1493,19 +1496,19 @@
       <c r="B6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="37"/>
-      <c r="E6" s="42" t="s">
+      <c r="D6" s="53"/>
+      <c r="E6" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="69"/>
       <c r="G6" s="54" t="s">
         <v>16</v>
       </c>
       <c r="H6" s="55"/>
-      <c r="I6" s="46"/>
+      <c r="I6" s="59"/>
       <c r="J6" s="15" t="s">
         <v>24</v>
       </c>
@@ -1514,18 +1517,18 @@
       <c r="B7" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
       <c r="G7" s="54" t="s">
         <v>17</v>
       </c>
       <c r="H7" s="55"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="42" t="s">
+      <c r="I7" s="59"/>
+      <c r="J7" s="61" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1533,37 +1536,37 @@
       <c r="B8" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
       <c r="G8" s="56"/>
       <c r="H8" s="57"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="48"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="62"/>
     </row>
     <row r="9" spans="2:10" ht="18" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="34" t="s">
+      <c r="D9" s="51"/>
+      <c r="E9" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="35"/>
-      <c r="G9" s="34" t="s">
+      <c r="F9" s="51"/>
+      <c r="G9" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="35"/>
-      <c r="I9" s="49" t="s">
+      <c r="H9" s="51"/>
+      <c r="I9" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="52" t="s">
+      <c r="J9" s="66" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1589,8 +1592,8 @@
       <c r="H10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="50"/>
-      <c r="J10" s="53"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="67"/>
     </row>
     <row r="11" spans="2:10" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="12" t="s">
@@ -1614,7 +1617,7 @@
       <c r="H11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="51"/>
+      <c r="I11" s="65"/>
       <c r="J11" s="8" t="s">
         <v>40</v>
       </c>
@@ -1657,16 +1660,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H8"/>
-    <mergeCell ref="I5:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="E9:F9"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E4:F4"/>
@@ -1676,6 +1669,16 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F8"/>
+    <mergeCell ref="I5:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1687,7 +1690,7 @@
   <dimension ref="B1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1701,19 +1704,19 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="60"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="76"/>
     </row>
     <row r="3" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
@@ -1779,40 +1782,40 @@
       <c r="K4" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="L4" s="62" t="s">
+      <c r="L4" s="33" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="69" t="s">
+      <c r="C5" s="39"/>
+      <c r="D5" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="E5" s="70" t="s">
+      <c r="E5" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="F5" s="70" t="s">
+      <c r="F5" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="G5" s="70" t="s">
+      <c r="G5" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="70" t="s">
+      <c r="H5" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="I5" s="71">
+      <c r="I5" s="42">
         <v>44615</v>
       </c>
-      <c r="J5" s="71">
+      <c r="J5" s="42">
         <v>44655</v>
       </c>
-      <c r="K5" s="68" t="s">
+      <c r="K5" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="L5" s="72" t="s">
+      <c r="L5" s="43" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1847,7 +1850,7 @@
       <c r="K6" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="L6" s="62"/>
+      <c r="L6" s="33"/>
     </row>
     <row r="7" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="29" t="s">
@@ -1880,55 +1883,55 @@
       <c r="K7" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="L7" s="62"/>
+      <c r="L7" s="33"/>
     </row>
     <row r="8" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="68" t="s">
+      <c r="C8" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="69" t="s">
+      <c r="D8" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="E8" s="70" t="s">
+      <c r="E8" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="70" t="s">
+      <c r="F8" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="G8" s="70"/>
-      <c r="H8" s="70" t="s">
+      <c r="G8" s="41"/>
+      <c r="H8" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="I8" s="71">
+      <c r="I8" s="42">
         <v>44703</v>
       </c>
-      <c r="J8" s="71"/>
-      <c r="K8" s="68"/>
-      <c r="L8" s="72"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="43"/>
     </row>
     <row r="9" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="73"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="65" t="s">
+      <c r="B9" s="44"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="66" t="s">
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="I9" s="74">
+      <c r="I9" s="45">
         <v>44615</v>
       </c>
-      <c r="J9" s="66"/>
-      <c r="K9" s="64" t="s">
+      <c r="J9" s="37"/>
+      <c r="K9" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="L9" s="75" t="s">
+      <c r="L9" s="46" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1961,7 +1964,7 @@
       <c r="K10" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="L10" s="62" t="s">
+      <c r="L10" s="33" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1994,36 +1997,36 @@
       <c r="K11" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="L11" s="62" t="s">
+      <c r="L11" s="33" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="68" t="s">
+      <c r="C12" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="69" t="s">
+      <c r="D12" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="70" t="s">
+      <c r="E12" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="70" t="s">
+      <c r="F12" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="70"/>
-      <c r="H12" s="70" t="s">
+      <c r="G12" s="41"/>
+      <c r="H12" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="I12" s="71">
+      <c r="I12" s="42">
         <v>44703</v>
       </c>
-      <c r="J12" s="71"/>
-      <c r="K12" s="68"/>
-      <c r="L12" s="72"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="43"/>
     </row>
     <row r="13" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="29" t="s">
@@ -2054,7 +2057,7 @@
       <c r="K13" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="L13" s="62" t="s">
+      <c r="L13" s="33" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2087,34 +2090,36 @@
       <c r="K14" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="L14" s="62" t="s">
+      <c r="L14" s="33" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="15" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="68" t="s">
+      <c r="C15" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="69"/>
-      <c r="E15" s="70" t="s">
+      <c r="D15" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="70" t="s">
+      <c r="F15" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="G15" s="70"/>
-      <c r="H15" s="70" t="s">
+      <c r="G15" s="41"/>
+      <c r="H15" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="I15" s="71">
+      <c r="I15" s="42">
         <v>44703</v>
       </c>
-      <c r="J15" s="70"/>
-      <c r="K15" s="68"/>
-      <c r="L15" s="72"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="43"/>
     </row>
     <row r="16" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="29" t="s">
@@ -2141,13 +2146,13 @@
       </c>
       <c r="J16" s="24"/>
       <c r="K16" s="31"/>
-      <c r="L16" s="62"/>
+      <c r="L16" s="33"/>
     </row>
     <row r="17" spans="2:12" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="61" t="s">
+      <c r="C17" s="32" t="s">
         <v>56</v>
       </c>
       <c r="D17" s="28" t="s">
@@ -2163,12 +2168,12 @@
       <c r="H17" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="I17" s="76">
+      <c r="I17" s="47">
         <v>44703</v>
       </c>
       <c r="J17" s="25"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="63"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
mise a jour des taches
</commit_message>
<xml_diff>
--- a/Matlab_Contenu_Detaille.xlsx
+++ b/Matlab_Contenu_Detaille.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marion\Desktop\Github\MATLAB_projet_echantillonage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\Github\MATLAB_projet_echantillonage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1B571B-22B2-4552-8909-3193BE3C3692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A4EE1B-6351-4DF0-8E21-1637D2E7131C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planning" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="107">
   <si>
     <t>Environnement Matlab et types de fenêtres (Workspace, fenêtre de commande, …)</t>
   </si>
@@ -361,6 +361,9 @@
   </si>
   <si>
     <t xml:space="preserve">Validation de la fonction interpolation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correction globale du code </t>
   </si>
 </sst>
 </file>
@@ -1056,6 +1059,40 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1064,40 +1101,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1485,7 +1488,7 @@
         <v>15</v>
       </c>
       <c r="H5" s="53"/>
-      <c r="I5" s="58" t="s">
+      <c r="I5" s="61" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="14" t="s">
@@ -1500,15 +1503,15 @@
         <v>9</v>
       </c>
       <c r="D6" s="53"/>
-      <c r="E6" s="61" t="s">
+      <c r="E6" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="69"/>
-      <c r="G6" s="54" t="s">
+      <c r="F6" s="55"/>
+      <c r="G6" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="55"/>
-      <c r="I6" s="59"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="62"/>
       <c r="J6" s="15" t="s">
         <v>24</v>
       </c>
@@ -1517,18 +1520,18 @@
       <c r="B7" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="68" t="s">
+      <c r="C7" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="69"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="54" t="s">
+      <c r="D7" s="55"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="55"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="61" t="s">
+      <c r="H7" s="71"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="58" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1536,16 +1539,16 @@
       <c r="B8" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="70" t="s">
+      <c r="C8" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="71"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="62"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="64"/>
     </row>
     <row r="9" spans="2:10" ht="18" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
@@ -1563,10 +1566,10 @@
         <v>37</v>
       </c>
       <c r="H9" s="51"/>
-      <c r="I9" s="63" t="s">
+      <c r="I9" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="66" t="s">
+      <c r="J9" s="68" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1592,8 +1595,8 @@
       <c r="H10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="64"/>
-      <c r="J10" s="67"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="69"/>
     </row>
     <row r="11" spans="2:10" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="12" t="s">
@@ -1617,7 +1620,7 @@
       <c r="H11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="65"/>
+      <c r="I11" s="67"/>
       <c r="J11" s="8" t="s">
         <v>40</v>
       </c>
@@ -1660,6 +1663,16 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H8"/>
+    <mergeCell ref="I5:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="E9:F9"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E4:F4"/>
@@ -1669,16 +1682,6 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F8"/>
-    <mergeCell ref="I5:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1689,8 +1692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{883C19B0-CCFC-48B4-9B7E-E834A0101326}">
   <dimension ref="B1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2048,12 +2051,14 @@
         <v>94</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I13" s="26">
         <v>44691</v>
       </c>
-      <c r="J13" s="24"/>
+      <c r="J13" s="26">
+        <v>44703</v>
+      </c>
       <c r="K13" s="31" t="s">
         <v>100</v>
       </c>
@@ -2081,12 +2086,14 @@
         <v>87</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I14" s="26">
         <v>44691</v>
       </c>
-      <c r="J14" s="24"/>
+      <c r="J14" s="26">
+        <v>44703</v>
+      </c>
       <c r="K14" s="31" t="s">
         <v>84</v>
       </c>
@@ -2112,7 +2119,7 @@
       </c>
       <c r="G15" s="41"/>
       <c r="H15" s="41" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I15" s="42">
         <v>44703</v>
@@ -2139,14 +2146,20 @@
         <v>71</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I16" s="26">
         <v>44703</v>
       </c>
-      <c r="J16" s="24"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="33"/>
+      <c r="J16" s="26">
+        <v>44703</v>
+      </c>
+      <c r="K16" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="L16" s="33" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="17" spans="2:12" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="30" t="s">

</xml_diff>